<commit_message>
'Updates requirement check & correct know db error'
</commit_message>
<xml_diff>
--- a/Data/course_backup.xlsx
+++ b/Data/course_backup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Columbia University\Courses\CMOS6156 Cloud Computing\Columbia-Course-Recommendation-System\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Columbia University\Courses\CMOS6156 Cloud Computing\Columbia-Course-Recommendation-System\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25582A12-019D-4921-AAB0-EDB8894A82F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5441741C-57F0-429B-8B37-A666797F77B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="course" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="707">
   <si>
     <t>Course</t>
   </si>
@@ -2138,12 +2138,15 @@
   </si>
   <si>
     <t>TPCS-ELEC &amp; COMPUT ENGINE</t>
+  </si>
+  <si>
+    <t>COMS4705W002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2984,11 +2987,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="A292" sqref="A292:XFD292"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3742,7 +3745,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>706</v>
       </c>
       <c r="B24" t="s">
         <v>96</v>

</xml_diff>